<commit_message>
top site build / mobild not functioning
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexe\Documents\GitHub\novelupdates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexe\Documents\GitHub\novelupdates\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{240A86A5-1A6C-4EDF-9ED9-1BBE92F593FF}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C14B0F9-AF3A-4AE1-A1B9-FCC20C79D5B6}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="8895" xr2:uid="{3F6B1CEE-64E8-429B-9AE1-2BAA8EC1B4E0}"/>
   </bookViews>
@@ -179,7 +179,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -194,6 +194,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13.5"/>
+      <color rgb="FF000000"/>
+      <name val="Space mono"/>
     </font>
   </fonts>
   <fills count="5">
@@ -234,13 +240,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -559,12 +568,12 @@
   <dimension ref="A1:P27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:H1"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:16">
       <c r="E1" t="s">
         <v>43</v>
       </c>
@@ -590,7 +599,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:16">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -610,7 +619,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:16">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
@@ -630,7 +639,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:16">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -650,7 +659,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:16">
       <c r="A5" t="s">
         <v>42</v>
       </c>
@@ -667,7 +676,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:16">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -687,7 +696,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:16">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -707,7 +716,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:16">
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
@@ -718,7 +727,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:16">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -738,7 +747,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:16">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -758,7 +767,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:16">
       <c r="A11" s="4" t="s">
         <v>8</v>
       </c>
@@ -778,7 +787,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:16">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -798,7 +807,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:16">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -818,7 +827,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:16">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -829,7 +838,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:16">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -840,7 +849,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:16">
       <c r="A16" s="4" t="s">
         <v>13</v>
       </c>
@@ -851,7 +860,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:10">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -862,7 +871,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:10">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -873,7 +882,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:10" ht="17.25">
       <c r="A20" s="5" t="s">
         <v>16</v>
       </c>
@@ -883,8 +892,9 @@
       <c r="H20" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="J20" s="6"/>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21" t="s">
         <v>17</v>
       </c>
@@ -895,7 +905,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:10">
       <c r="A22" t="s">
         <v>18</v>
       </c>
@@ -906,7 +916,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:10">
       <c r="A23" t="s">
         <v>19</v>
       </c>
@@ -917,7 +927,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:10">
       <c r="A24" t="s">
         <v>20</v>
       </c>
@@ -928,7 +938,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:10">
       <c r="A25" t="s">
         <v>21</v>
       </c>
@@ -939,7 +949,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:10">
       <c r="A26" t="s">
         <v>22</v>
       </c>
@@ -950,7 +960,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:10">
       <c r="A27" t="s">
         <v>46</v>
       </c>
@@ -963,6 +973,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -975,9 +986,9 @@
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8">
       <c r="E1" t="s">
         <v>43</v>
       </c>
@@ -991,7 +1002,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -1002,7 +1013,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -1013,7 +1024,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -1024,7 +1035,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -1035,7 +1046,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>33</v>
       </c>
@@ -1046,7 +1057,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -1057,7 +1068,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>35</v>
       </c>
@@ -1068,7 +1079,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>36</v>
       </c>

</xml_diff>